<commit_message>
Removed basic blue color with banner image for each site Added icons to static and added them on contact and home
</commit_message>
<xml_diff>
--- a/TwitterSentimentAnalyser/TSentimentAnalyser/static/xlsx/raw_tweets.xlsx
+++ b/TwitterSentimentAnalyser/TSentimentAnalyser/static/xlsx/raw_tweets.xlsx
@@ -511,57 +511,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RT @mi6rogue: This is the @Conservatives newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. https://t.co/XiXc…</t>
+          <t>RT @gDesFaits: #BIDEN sait bien s'entourer... #pedophilie
+Jerry Harris, star de l'émission Netflix « Cheer » et ancien substitut de la cam…</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.339198595254215e+18</v>
+        <v>1.339229134069916e+18</v>
       </c>
       <c r="D2" t="n">
         <v>140</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44181.55555555555</v>
+        <v>44181.63982638889</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>35221272</v>
+        <v>1.077271244964315e+18</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>gothamcity56</t>
+          <t>botduSEXE</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>668</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>West Sussex</t>
-        </is>
-      </c>
+        <v>1850</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @mi6rogue: This is the @Conservatives newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. https://t.co/XiXc… </t>
+          <t xml:space="preserve">RT @gDesFaits: #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This is the  newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. …</t>
+          <t xml:space="preserve"> #BIDEN sait bien s'entourer... #pedophilie  Jerry Harris, star de l'émission Netflix « Cheer » et ancien substitut de la cam…</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This is the  newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. … </t>
+          <t xml:space="preserve"> #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @mi6rogue: This is the @Conservatives newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. … </t>
+          <t xml:space="preserve">RT @gDesFaits: #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
         </is>
       </c>
     </row>
@@ -571,17 +568,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RT @bitcoinconnect: PS5 beats toilet paper, face masks in Google’s top searches of 2020 ***RESTOCKS*** SEE MORE HERE ==&amp;gt; https://t.co/pjC7m…</t>
+          <t>Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am… https://t.co/2uhi1nNOjP</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.339198593580806e+18</v>
+        <v>1.339229096069349e+18</v>
       </c>
       <c r="D3" t="n">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44181.55555555555</v>
+        <v>44181.63972222222</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -589,35 +586,35 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.332740896199238e+18</v>
+        <v>1352572483</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>XboxRetweeter</t>
+          <t>sethrow991</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>396</v>
+        <v>162</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @bitcoinconnect: PS5 beats toilet paper, face masks in Google’s top searches of 2020 ***RESTOCKS*** SEE MORE HERE ==&amp;gt; https://t.co/pjC7m… </t>
+          <t xml:space="preserve">Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am… https://t.co/2uhi1nNOjP </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PS5 beats toilet paper, face masks in Google’s top searches of 2020 ***RESTOCKS*** SEE MORE HERE ==&amp;gt; …</t>
+          <t xml:space="preserve">Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am… </t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PS5 beats toilet paper, face masks in Google’s top searches of 2020 ***RESTOCKS*** SEE MORE HERE ==&amp;gt; … </t>
+          <t xml:space="preserve">Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am…  </t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @bitcoinconnect: PS5 beats toilet paper, face masks in Google’s top searches of 2020 ***RESTOCKS*** SEE MORE HERE ==&amp;gt; … </t>
+          <t xml:space="preserve">Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am…  </t>
         </is>
       </c>
     </row>
@@ -627,17 +624,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RT @bitcoinconnect: PS5 vs. Xbox Series X: why is the PS5 outperforming the next-gen Xbox? SEE MORE HERE ==&amp;gt; https://t.co/uTKq3jCQuw #ninte…</t>
+          <t>RT @in_pubs: If you need a pick me up today....
+Just think....
+At this very moment @realDonaldTrump and his lawyers. 
+Are scrambling to…</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.339198593564111e+18</v>
+        <v>1.339229085529231e+18</v>
       </c>
       <c r="D4" t="n">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44181.55555555555</v>
+        <v>44181.63969907408</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -645,35 +645,35 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1.332740896199238e+18</v>
+        <v>8.225891453359555e+17</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>XboxRetweeter</t>
+          <t>Loiskane1202</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>396</v>
+        <v>154</v>
       </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @bitcoinconnect: PS5 vs. Xbox Series X: why is the PS5 outperforming the next-gen Xbox? SEE MORE HERE ==&amp;gt; https://t.co/uTKq3jCQuw #ninte… </t>
+          <t xml:space="preserve">RT @in_pubs: If you need a pick me up today....Just think....At this very moment @realDonaldTrump and his lawyers. Are scrambling to… </t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PS5 vs. Xbox Series X: why is the PS5 outperforming the next-gen Xbox? SEE MORE HERE ==&amp;gt;  #ninte…</t>
+          <t xml:space="preserve"> If you need a pick me up today....  Just think....  At this very moment  and his lawyers.   Are scrambling to…</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> PS5 vs. Xbox Series X: why is the PS5 outperforming the next-gen Xbox? SEE MORE HERE ==&amp;gt;  #ninte… </t>
+          <t xml:space="preserve"> If you need a pick me up today....Just think....At this very moment  and his lawyers. Are scrambling to… </t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @bitcoinconnect: PS5 vs. Xbox Series X: why is the PS5 outperforming the next-gen Xbox? SEE MORE HERE ==&amp;gt;  #ninte… </t>
+          <t xml:space="preserve">RT @in_pubs: If you need a pick me up today....Just think....At this very moment @realDonaldTrump and his lawyers. Are scrambling to… </t>
         </is>
       </c>
     </row>
@@ -683,17 +683,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RT @cowards_are_us: U WOULD THINK @senatemajldr &amp;amp; @GOPLeader WOULD RUSH IN &amp;amp; PROTECT OUR COUNTRY AS #Trump's CRIMINAL LIFE &amp;amp; BUNGLING FAILU…</t>
+          <t>Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is… https://t.co/LjFKYUVHx9</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.33919858450441e+18</v>
+        <v>1.339229062091444e+18</v>
       </c>
       <c r="D5" t="n">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44181.55553240741</v>
+        <v>44181.63962962963</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -701,39 +701,35 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>7.369050005935759e+17</v>
+        <v>8.39482284759724e+17</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>cowards_are_us</t>
+          <t>trumpfreakout</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>10341</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Chicago, IL</t>
-        </is>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @cowards_are_us: U WOULD THINK @senatemajldr &amp;amp; @GOPLeader WOULD RUSH IN &amp;amp; PROTECT OUR COUNTRY AS #Trump's CRIMINAL LIFE &amp;amp; BUNGLING FAILU… </t>
+          <t xml:space="preserve">Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is… https://t.co/LjFKYUVHx9 </t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> U WOULD THINK  &amp;amp;  WOULD RUSH IN &amp;amp; PROTECT OUR COUNTRY AS #Trump's CRIMINAL LIFE &amp;amp; BUNGLING FAILU…</t>
+          <t xml:space="preserve">Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is… </t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> U WOULD THINK  &amp;amp;  WOULD RUSH IN &amp;amp; PROTECT OUR COUNTRY AS #Trump's CRIMINAL LIFE &amp;amp; BUNGLING FAILU… </t>
+          <t xml:space="preserve">Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is…  </t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @cowards_are_us: U WOULD THINK @senatemajldr &amp;amp; @GOPLeader WOULD RUSH IN &amp;amp; PROTECT OUR COUNTRY AS #Trump's CRIMINAL LIFE &amp;amp; BUNGLING FAILU… </t>
+          <t xml:space="preserve">Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is…  </t>
         </is>
       </c>
     </row>
@@ -743,18 +739,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Read these breaking headlines at https://t.co/8DcwIEtHo8.
-#voteinorout #trump #biden #loeffler #perdue #thebraves… https://t.co/C29XgmjQba</t>
+          <t>@ThomTillis @Perduesenate @KLoeffler Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d… https://t.co/tPSF80ZcfZ</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.339198582201717e+18</v>
+        <v>1.339229040096457e+18</v>
       </c>
       <c r="D6" t="n">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44181.55552083333</v>
+        <v>44181.63957175926</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -762,39 +757,39 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1.055578127223738e+18</v>
+        <v>416363599</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>voteinorout</t>
+          <t>GeneKelsey</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>2418</v>
+        <v>113</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>New York, USA</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Read these breaking headlines at https://t.co/8DcwIEtHo8.#voteinorout #trump #biden #loeffler #perdue #thebraves… https://t.co/C29XgmjQba </t>
+          <t xml:space="preserve">@ThomTillis @Perduesenate @KLoeffler Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d… https://t.co/tPSF80ZcfZ </t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Read these breaking headlines at   #voteinorout #trump #biden #loeffler #perdue #thebraves… </t>
+          <t xml:space="preserve">   Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d… </t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Read these breaking headlines at #voteinorout #trump #biden #loeffler #perdue #thebraves…  </t>
+          <t xml:space="preserve">   Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d…  </t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Read these breaking headlines at #voteinorout #trump #biden #loeffler #perdue #thebraves…  </t>
+          <t xml:space="preserve">@ThomTillis @Perduesenate @KLoeffler Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d…  </t>
         </is>
       </c>
     </row>
@@ -804,17 +799,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RT @mi6rogue: This is the @Conservatives newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. https://t.co/XiXc…</t>
+          <t>IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENS
+https://t.co/dumJMhzp02</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.339198579982922e+18</v>
+        <v>1.339229035797352e+18</v>
       </c>
       <c r="D7" t="n">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44181.55552083333</v>
+        <v>44181.63956018518</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -822,39 +818,39 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>124296126</v>
+        <v>90272103</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Gordy_Mc1ntosh</t>
+          <t>gezgintrk</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>10884</v>
+        <v>12308</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>European Union 🇪🇺</t>
+          <t>Turkey / İstanbul</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @mi6rogue: This is the @Conservatives newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. https://t.co/XiXc… </t>
+          <t xml:space="preserve">IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENShttps://t.co/dumJMhzp02 </t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This is the  newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. …</t>
+          <t xml:space="preserve">IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENS </t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This is the  newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. … </t>
+          <t xml:space="preserve">IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENS </t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @mi6rogue: This is the @Conservatives newsletter detailing how Tories can learn from #Trump and “weaponise” fake news. … </t>
+          <t xml:space="preserve">IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENS </t>
         </is>
       </c>
     </row>
@@ -864,58 +860,58 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>#TwitterPoll 
-It's an easy argument that #Trump has violated @Twitter rules enough in the past to expect he will c… https://t.co/puNHNpxI7I</t>
+          <t>RT @gDesFaits: #BIDEN sait bien s'entourer... #pedophilie
+Jerry Harris, star de l'émission Netflix « Cheer » et ancien substitut de la cam…</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.339198565269328e+18</v>
+        <v>1.339229026062393e+18</v>
       </c>
       <c r="D8" t="n">
         <v>140</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>44181.55547453704</v>
+        <v>44181.63953703704</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>567210744</v>
+        <v>7.16571320574677e+17</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>EndAllSuffering</t>
+          <t>JePPauwels</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>6832</v>
+        <v>154</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Deep River, Connecticut, USA</t>
+          <t>Hainaut, Belgique</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t xml:space="preserve">#TwitterPoll It's an easy argument that #Trump has violated @Twitter rules enough in the past to expect he will c… https://t.co/puNHNpxI7I </t>
+          <t xml:space="preserve">RT @gDesFaits: #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve">#TwitterPoll   It's an easy argument that #Trump has violated  rules enough in the past to expect he will c… </t>
+          <t xml:space="preserve"> #BIDEN sait bien s'entourer... #pedophilie  Jerry Harris, star de l'émission Netflix « Cheer » et ancien substitut de la cam…</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t xml:space="preserve">#TwitterPoll It's an easy argument that #Trump has violated  rules enough in the past to expect he will c…  </t>
+          <t xml:space="preserve"> #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t xml:space="preserve">#TwitterPoll It's an easy argument that #Trump has violated @Twitter rules enough in the past to expect he will c…  </t>
+          <t xml:space="preserve">RT @gDesFaits: #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
         </is>
       </c>
     </row>
@@ -925,57 +921,54 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RT @drybonescartoon: Is American Democracy Out of Control? #Trump #Biden #BidenHarris2020 #MAGA #Trump2024 #Trumpism https://t.co/WCkCrP7lmw</t>
+          <t>RT @MarteauOlivier: Quand #Obama a été réélu en 2012, il avait perdu 3 millions de voix par rapport à son élection en 2008.
+#Trump lui a ga…</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.339198554062139e+18</v>
+        <v>1.339228998992359e+18</v>
       </c>
       <c r="D9" t="n">
         <v>140</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44181.55545138889</v>
+        <v>44181.63945601852</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>820064220</v>
+        <v>3138038768</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>ZackT613</t>
+          <t>Randy64_fr</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>223</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Brooklyn, NY</t>
-        </is>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @drybonescartoon: Is American Democracy Out of Control? #Trump #Biden #BidenHarris2020 #MAGA #Trump2024 #Trumpism https://t.co/WCkCrP7lmw </t>
+          <t xml:space="preserve">RT @MarteauOlivier: When #Obama was re-elected in 2012, he had lost 3 million votes compared to his election in 2008. # Trump gave him ... </t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Is American Democracy Out of Control? #Trump #Biden #BidenHarris2020 #MAGA #Trump2024 #Trumpism </t>
+          <t xml:space="preserve"> Quand #Obama a été réélu en 2012, il avait perdu 3 millions de voix par rapport à son élection en 2008. #Trump lui a ga…</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Is American Democracy Out of Control? #Trump #Biden #BidenHarris2020 #MAGA #Trump2024 #Trumpism  </t>
+          <t xml:space="preserve"> When #Obama was re-elected in 2012, he had lost 3 million votes compared to his election in 2008. # Trump gave him ... </t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @drybonescartoon: Is American Democracy Out of Control? #Trump #Biden #BidenHarris2020 #MAGA #Trump2024 #Trumpism  </t>
+          <t xml:space="preserve">RT @MarteauOlivier: When #Obama was re-elected in 2012, he had lost 3 million votes compared to his election in 2008. # Trump gave him ... </t>
         </is>
       </c>
     </row>
@@ -985,17 +978,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>@JakeSherman @BretBaier Remember Dems stellar “Obstruction of Justice” claims against #Trump and thier basis for th… https://t.co/0nbPdtSGeo</t>
+          <t>RT @Susan10515068: Trump fucking lost and there is nothing you can do...
+#TrumpTheFool 
+#Trump 
+#PsychoTrump https://t.co/wWvLaJzEig</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.339198550572413e+18</v>
+        <v>1.339228997310407e+18</v>
       </c>
       <c r="D10" t="n">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44181.55543981482</v>
+        <v>44181.63945601852</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1003,39 +999,35 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>111665923</v>
+        <v>900977000</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>AndeyR</t>
+          <t>Cradd4Teresa</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>6949</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Michigan</t>
-        </is>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t xml:space="preserve">@JakeSherman @BretBaier Remember Dems stellar “Obstruction of Justice” claims against #Trump and thier basis for th… https://t.co/0nbPdtSGeo </t>
+          <t xml:space="preserve">RT @Susan10515068: Trump fucking lost and there is nothing you can do...#TrumpTheFool #Trump #PsychoTrump https://t.co/wWvLaJzEig </t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Remember Dems stellar “Obstruction of Justice” claims against #Trump and thier basis for th… </t>
+          <t xml:space="preserve"> Trump fucking lost and there is nothing you can do... #TrumpTheFool  #Trump  #PsychoTrump </t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t xml:space="preserve">  Remember Dems stellar “Obstruction of Justice” claims against #Trump and thier basis for th…  </t>
+          <t xml:space="preserve"> Trump fucking lost and there is nothing you can do...#TrumpTheFool #Trump #PsychoTrump  </t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t xml:space="preserve">@JakeSherman @BretBaier Remember Dems stellar “Obstruction of Justice” claims against #Trump and thier basis for th…  </t>
+          <t xml:space="preserve">RT @Susan10515068: Trump fucking lost and there is nothing you can do...#TrumpTheFool #Trump #PsychoTrump  </t>
         </is>
       </c>
     </row>
@@ -1045,17 +1037,19 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>@marcorubio Mysterious gap in #COVID19 deaths appeared in #Florida before the presidential #Election2020… https://t.co/oLcN1m47XU</t>
+          <t>@realDonaldTrump @FoxNews #Trump is irrelevant. 
+Ignore the insane ramblings of #PsychoTrump #25th 
+#Georgia deser… https://t.co/RYfE4nwE8B</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.339198546558542e+18</v>
+        <v>1.339228980302537e+18</v>
       </c>
       <c r="D11" t="n">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44181.55542824074</v>
+        <v>44181.63940972222</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1063,39 +1057,39 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>18379569</v>
+        <v>1.173506442491519e+18</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Layofflist</t>
+          <t>LeeSaunders72</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>3018</v>
+        <v>1179</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Rochester, NY</t>
+          <t>Leeds/Manchester/London, UK</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t xml:space="preserve">@marcorubio Mysterious gap in #COVID19 deaths appeared in #Florida before the presidential #Election2020… https://t.co/oLcN1m47XU </t>
+          <t xml:space="preserve">@realDonaldTrump @FoxNews #Trump is irrelevant. Ignore the insane ramblings of #PsychoTrump #25th #Georgia deser… https://t.co/RYfE4nwE8B </t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mysterious gap in #COVID19 deaths appeared in #Florida before the presidential #Election2020… </t>
+          <t xml:space="preserve">  #Trump is irrelevant.  Ignore the insane ramblings of #PsychoTrump #25th   #Georgia deser… </t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mysterious gap in #COVID19 deaths appeared in #Florida before the presidential #Election2020…  </t>
+          <t xml:space="preserve">  #Trump is irrelevant. Ignore the insane ramblings of #PsychoTrump #25th #Georgia deser…  </t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t xml:space="preserve">@marcorubio Mysterious gap in #COVID19 deaths appeared in #Florida before the presidential #Election2020…  </t>
+          <t xml:space="preserve">@realDonaldTrump @FoxNews #Trump is irrelevant. Ignore the insane ramblings of #PsychoTrump #25th #Georgia deser…  </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed gif and replaced with mp4 format
</commit_message>
<xml_diff>
--- a/TwitterSentimentAnalyser/TSentimentAnalyser/static/xlsx/raw_tweets.xlsx
+++ b/TwitterSentimentAnalyser/TSentimentAnalyser/static/xlsx/raw_tweets.xlsx
@@ -511,54 +511,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RT @gDesFaits: #BIDEN sait bien s'entourer... #pedophilie
-Jerry Harris, star de l'émission Netflix « Cheer » et ancien substitut de la cam…</t>
+          <t>xmas came early 
+thank you #Bitcoin $BTC</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.339229134069916e+18</v>
+        <v>1.339281910548341e+18</v>
       </c>
       <c r="D2" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44181.63982638889</v>
+        <v>44181.78546296297</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1.077271244964315e+18</v>
+        <v>82204541</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>botduSEXE</t>
+          <t>GreatCoinhodlio</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1850</v>
+        <v>107</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @gDesFaits: #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
+          <t xml:space="preserve">xmas came early thank you #Bitcoin $BTC </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #BIDEN sait bien s'entourer... #pedophilie  Jerry Harris, star de l'émission Netflix « Cheer » et ancien substitut de la cam…</t>
+          <t>xmas came early  thank you #Bitcoin $BTC</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
+          <t xml:space="preserve">xmas came early thank you #Bitcoin $BTC </t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @gDesFaits: #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
+          <t xml:space="preserve">xmas came early thank you #Bitcoin $BTC </t>
         </is>
       </c>
     </row>
@@ -568,53 +568,53 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am… https://t.co/2uhi1nNOjP</t>
+          <t>@Kneteknilch @mspro DIE Lösung für alles...Das habe ich auch nie behauptet. Dennoch wird Bitcoin nicht durch irgend… https://t.co/t6zfoL1WvH</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.339229096069349e+18</v>
+        <v>1.339281909587775e+18</v>
       </c>
       <c r="D3" t="n">
         <v>140</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44181.63972222222</v>
+        <v>44181.78546296297</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>de</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1352572483</v>
+        <v>1.311435962925429e+18</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>sethrow991</t>
+          <t>HodlingSquirrel</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>162</v>
+        <v>6</v>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am… https://t.co/2uhi1nNOjP </t>
+          <t xml:space="preserve">@Kneteknilch @mspro THE solution for everything ... I never said that. Still, Bitcoin is not made by any ... https://t.co/t6zfoL1WvH </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am… </t>
+          <t xml:space="preserve">  DIE Lösung für alles...Das habe ich auch nie behauptet. Dennoch wird Bitcoin nicht durch irgend… </t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am…  </t>
+          <t xml:space="preserve">  THE solution for everything ... I never said that. Still, Bitcoin is not made by any ...  </t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Abusing #Republican Leaders #Media #Trump #Facebook America Law Government Sports Entertainment health Education Am…  </t>
+          <t xml:space="preserve">@Kneteknilch @mspro THE solution for everything ... I never said that. Still, Bitcoin is not made by any ...  </t>
         </is>
       </c>
     </row>
@@ -624,20 +624,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RT @in_pubs: If you need a pick me up today....
-Just think....
-At this very moment @realDonaldTrump and his lawyers. 
-Are scrambling to…</t>
+          <t>This truly aged well.  #Bitcoin https://t.co/2dgOjMAjJe</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.339229085529231e+18</v>
+        <v>1.339281909512286e+18</v>
       </c>
       <c r="D4" t="n">
-        <v>139</v>
+        <v>55</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44181.63969907408</v>
+        <v>44181.78546296297</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -645,35 +642,39 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>8.225891453359555e+17</v>
+        <v>19603980</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Loiskane1202</t>
+          <t>GlenACooper</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>154</v>
-      </c>
-      <c r="J4" t="inlineStr"/>
+        <v>101</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Reston, VA</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @in_pubs: If you need a pick me up today....Just think....At this very moment @realDonaldTrump and his lawyers. Are scrambling to… </t>
+          <t xml:space="preserve">This truly aged well.  #Bitcoin https://t.co/2dgOjMAjJe </t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> If you need a pick me up today....  Just think....  At this very moment  and his lawyers.   Are scrambling to…</t>
+          <t xml:space="preserve">This truly aged well.  #Bitcoin </t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> If you need a pick me up today....Just think....At this very moment  and his lawyers. Are scrambling to… </t>
+          <t xml:space="preserve">This truly aged well.  #Bitcoin  </t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @in_pubs: If you need a pick me up today....Just think....At this very moment @realDonaldTrump and his lawyers. Are scrambling to… </t>
+          <t xml:space="preserve">This truly aged well.  #Bitcoin  </t>
         </is>
       </c>
     </row>
@@ -683,53 +684,54 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is… https://t.co/LjFKYUVHx9</t>
+          <t>#16Dic La policía de Trinidad y Tobago. maltratando y Agrediendo  a Migrantes Venezolanos 
+ Es inaceptable que los… https://t.co/U9JJdOks6R</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.339229062091444e+18</v>
+        <v>1.339281905062195e+18</v>
       </c>
       <c r="D5" t="n">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44181.63962962963</v>
+        <v>44181.78545138889</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>es</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>8.39482284759724e+17</v>
+        <v>430205402</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>trumpfreakout</t>
+          <t>VzlaUfo</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>67</v>
+        <v>2084</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is… https://t.co/LjFKYUVHx9 </t>
+          <t xml:space="preserve"># 16Dec Trinidad and Tobago Police. mistreating and attacking Venezuelan Migrants It is unacceptable that the… https://t.co/U9JJdOks6R </t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is… </t>
+          <t xml:space="preserve">#16Dic La policía de Trinidad y Tobago. maltratando y Agrediendo  a Migrantes Venezolanos   Es inaceptable que los… </t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is…  </t>
+          <t xml:space="preserve"># 16Dec Trinidad and Tobago Police. mistreating and attacking Venezuelan Migrants It is unacceptable that the…  </t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Oups another #freakout! #trump #fail realDonaldTrump: Perhaps the biggest difference between 2016 and 2020 is…  </t>
+          <t xml:space="preserve"># 16Dec Trinidad and Tobago Police. mistreating and attacking Venezuelan Migrants It is unacceptable that the…  </t>
         </is>
       </c>
     </row>
@@ -739,17 +741,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>@ThomTillis @Perduesenate @KLoeffler Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d… https://t.co/tPSF80ZcfZ</t>
+          <t>Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.339229040096457e+18</v>
+        <v>1.339281902096634e+18</v>
       </c>
       <c r="D6" t="n">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44181.63957175926</v>
+        <v>44181.78543981481</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -757,39 +759,39 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>416363599</v>
+        <v>1.259302062434578e+18</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>GeneKelsey</t>
+          <t>KOBOcrypto</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>California, USA</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t xml:space="preserve">@ThomTillis @Perduesenate @KLoeffler Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d… https://t.co/tPSF80ZcfZ </t>
+          <t xml:space="preserve">Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin </t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d… </t>
+          <t>Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve">   Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d…  </t>
+          <t xml:space="preserve">Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin </t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t xml:space="preserve">@ThomTillis @Perduesenate @KLoeffler Like the other #GOPTraitors, #Loeffler &amp;amp; #Perdue stood silently by as #Trump d…  </t>
+          <t xml:space="preserve">Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin </t>
         </is>
       </c>
     </row>
@@ -799,58 +801,58 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENS
-https://t.co/dumJMhzp02</t>
+          <t>RT @davidnathan: Humeur du jour chez les bitcoiners... 😁 https://t.co/nZbOGMwFTT
+#Bitcoin #BTC</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.339229035797352e+18</v>
+        <v>1.33928190054067e+18</v>
       </c>
       <c r="D7" t="n">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44181.63956018518</v>
+        <v>44181.78543981481</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>fr</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>90272103</v>
+        <v>1.321825428974297e+18</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>gezgintrk</t>
+          <t>crypto_actu_fr</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>12308</v>
+        <v>130</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Turkey / İstanbul</t>
+          <t xml:space="preserve">France </t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t xml:space="preserve">IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENShttps://t.co/dumJMhzp02 </t>
+          <t xml:space="preserve">RT @davidnathan: Mood of the day among bitcoiners ... 😁 https://t.co/nZbOGMwFTT#Bitcoin #BTC </t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t xml:space="preserve">IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENS </t>
+          <t xml:space="preserve"> Humeur du jour chez les bitcoiners... 😁   #Bitcoin #BTC</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t xml:space="preserve">IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENS </t>
+          <t xml:space="preserve"> Mood of the day among bitcoiners ... 😁 #Bitcoin #BTC </t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t xml:space="preserve">IN 2020, THE #TRUMP ADMINISTRATION DECLARED WAR ON DANCING TEENS </t>
+          <t xml:space="preserve">RT @davidnathan: Mood of the day among bitcoiners ... 😁 #Bitcoin #BTC </t>
         </is>
       </c>
     </row>
@@ -860,58 +862,53 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RT @gDesFaits: #BIDEN sait bien s'entourer... #pedophilie
-Jerry Harris, star de l'émission Netflix « Cheer » et ancien substitut de la cam…</t>
+          <t>@milyonerzihin @RealWorldCripto #Bitcoin 36500</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.339229026062393e+18</v>
+        <v>1.339281895562023e+18</v>
       </c>
       <c r="D8" t="n">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>44181.63953703704</v>
+        <v>44181.78542824074</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>und</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>7.16571320574677e+17</v>
+        <v>85309928</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>JePPauwels</t>
+          <t>r_tuynak</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>154</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Hainaut, Belgique</t>
-        </is>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @gDesFaits: #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
+          <t xml:space="preserve">@milyonerzihin @RealWorldCripto #Bitcoin 36500 </t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #BIDEN sait bien s'entourer... #pedophilie  Jerry Harris, star de l'émission Netflix « Cheer » et ancien substitut de la cam…</t>
+          <t xml:space="preserve">  #Bitcoin 36500</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
+          <t xml:space="preserve">  #Bitcoin 36500 </t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @gDesFaits: #BIDEN knows how to surround himself well ... #pedophiliaJerry Harris, star of the Netflix show "Cheer" and former cam substitute ... </t>
+          <t xml:space="preserve">@milyonerzihin @RealWorldCripto #Bitcoin 36500 </t>
         </is>
       </c>
     </row>
@@ -921,54 +918,53 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RT @MarteauOlivier: Quand #Obama a été réélu en 2012, il avait perdu 3 millions de voix par rapport à son élection en 2008.
-#Trump lui a ga…</t>
+          <t>RT @jsblokland: BREAKING! #Bitcoin spikes to above USD 20,000! https://t.co/olLH68WW7W</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.339228998992359e+18</v>
+        <v>1.339281894827938e+18</v>
       </c>
       <c r="D9" t="n">
-        <v>140</v>
+        <v>86</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44181.63945601852</v>
+        <v>44181.78542824074</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>3138038768</v>
+        <v>9.988576414546575e+17</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Randy64_fr</t>
+          <t>Sonal913</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>331</v>
+        <v>134</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @MarteauOlivier: When #Obama was re-elected in 2012, he had lost 3 million votes compared to his election in 2008. # Trump gave him ... </t>
+          <t xml:space="preserve">RT @jsblokland: BREAKING! #Bitcoin spikes to above USD 20,000! https://t.co/olLH68WW7W </t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quand #Obama a été réélu en 2012, il avait perdu 3 millions de voix par rapport à son élection en 2008. #Trump lui a ga…</t>
+          <t xml:space="preserve"> BREAKING! #Bitcoin spikes to above USD 20,000! </t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> When #Obama was re-elected in 2012, he had lost 3 million votes compared to his election in 2008. # Trump gave him ... </t>
+          <t xml:space="preserve"> BREAKING! #Bitcoin spikes to above USD 20,000!  </t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @MarteauOlivier: When #Obama was re-elected in 2012, he had lost 3 million votes compared to his election in 2008. # Trump gave him ... </t>
+          <t xml:space="preserve">RT @jsblokland: BREAKING! #Bitcoin spikes to above USD 20,000!  </t>
         </is>
       </c>
     </row>
@@ -978,56 +974,59 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>RT @Susan10515068: Trump fucking lost and there is nothing you can do...
-#TrumpTheFool 
-#Trump 
-#PsychoTrump https://t.co/wWvLaJzEig</t>
+          <t>RT @NamregNortlas: #16Dic
+#ANCSoberaniaYPaz
+#FelizMiercoles
+#BitCoin
+Día DEL Dibujante
+Copenhague
+#ExiliarAlReyYa #SOScolombiaddhh #Bolchev…</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.339228997310407e+18</v>
+        <v>1.339281892672205e+18</v>
       </c>
       <c r="D10" t="n">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44181.63945601852</v>
+        <v>44181.78541666667</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>es</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>900977000</v>
+        <v>1.318655859367547e+18</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Cradd4Teresa</t>
+          <t>DORISGa60466222</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>29</v>
+        <v>295</v>
       </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @Susan10515068: Trump fucking lost and there is nothing you can do...#TrumpTheFool #Trump #PsychoTrump https://t.co/wWvLaJzEig </t>
+          <t xml:space="preserve">RT @NamregNortlas: # 16Dec # ANCSoberaniaYPaz # FelizMiercoles # BitCoinDía DEL CartoonjaCopenhague # ExiliarAlReyYa #SOScolombiaddhh # Bolchev… </t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Trump fucking lost and there is nothing you can do... #TrumpTheFool  #Trump  #PsychoTrump </t>
+          <t xml:space="preserve"> #16Dic #ANCSoberaniaYPaz #FelizMiercoles #BitCoin Día DEL Dibujante Copenhague #ExiliarAlReyYa #SOScolombiaddhh #Bolchev…</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Trump fucking lost and there is nothing you can do...#TrumpTheFool #Trump #PsychoTrump  </t>
+          <t xml:space="preserve"> # 16Dec # ANCSoberaniaYPaz # FelizMiercoles # BitCoinDía DEL CartoonjaCopenhague # ExiliarAlReyYa #SOScolombiaddhh # Bolchev… </t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @Susan10515068: Trump fucking lost and there is nothing you can do...#TrumpTheFool #Trump #PsychoTrump  </t>
+          <t xml:space="preserve">RT @NamregNortlas: # 16Dec # ANCSoberaniaYPaz # FelizMiercoles # BitCoinDía DEL CartoonjaCopenhague # ExiliarAlReyYa #SOScolombiaddhh # Bolchev… </t>
         </is>
       </c>
     </row>
@@ -1037,19 +1036,18 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>@realDonaldTrump @FoxNews #Trump is irrelevant. 
-Ignore the insane ramblings of #PsychoTrump #25th 
-#Georgia deser… https://t.co/RYfE4nwE8B</t>
+          <t>The most important function of AITD chain is connecting the world!
+ #Ethereum #bitcoin #eth #uniswap #defi #gem… https://t.co/1bBsek11Ui</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.339228980302537e+18</v>
+        <v>1.339281891392893e+18</v>
       </c>
       <c r="D11" t="n">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44181.63940972222</v>
+        <v>44181.78541666667</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1057,39 +1055,35 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>1.173506442491519e+18</v>
+        <v>1.298076739369804e+18</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>LeeSaunders72</t>
+          <t>BlockchainAitd</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1179</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Leeds/Manchester/London, UK</t>
-        </is>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t xml:space="preserve">@realDonaldTrump @FoxNews #Trump is irrelevant. Ignore the insane ramblings of #PsychoTrump #25th #Georgia deser… https://t.co/RYfE4nwE8B </t>
+          <t xml:space="preserve">The most important function of AITD chain is connecting the world! #Ethereum #bitcoin #eth #uniswap #defi #gem… https://t.co/1bBsek11Ui </t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  #Trump is irrelevant.  Ignore the insane ramblings of #PsychoTrump #25th   #Georgia deser… </t>
+          <t xml:space="preserve">The most important function of AITD chain is connecting the world!  #Ethereum #bitcoin #eth #uniswap #defi #gem… </t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t xml:space="preserve">  #Trump is irrelevant. Ignore the insane ramblings of #PsychoTrump #25th #Georgia deser…  </t>
+          <t xml:space="preserve">The most important function of AITD chain is connecting the world! #Ethereum #bitcoin #eth #uniswap #defi #gem…  </t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t xml:space="preserve">@realDonaldTrump @FoxNews #Trump is irrelevant. Ignore the insane ramblings of #PsychoTrump #25th #Georgia deser…  </t>
+          <t xml:space="preserve">The most important function of AITD chain is connecting the world! #Ethereum #bitcoin #eth #uniswap #defi #gem…  </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed column names for df_short
</commit_message>
<xml_diff>
--- a/TwitterSentimentAnalyser/TSentimentAnalyser/static/xlsx/raw_tweets.xlsx
+++ b/TwitterSentimentAnalyser/TSentimentAnalyser/static/xlsx/raw_tweets.xlsx
@@ -511,18 +511,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>xmas came early 
-thank you #Bitcoin $BTC</t>
+          <t>RT @TribulationThe: TREASON by the Biden Crime Family!
+"Please Have Keys Made": Joe Biden Was Chinese Financier's "Office Mate" According…</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.339281910548341e+18</v>
+        <v>1.339313651711357e+18</v>
       </c>
       <c r="D2" t="n">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44181.78546296297</v>
+        <v>44181.87305555555</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -530,35 +530,39 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>82204541</v>
+        <v>22442937</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>GreatCoinhodlio</t>
+          <t>TheTybeeTimes</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>107</v>
-      </c>
-      <c r="J2" t="inlineStr"/>
+        <v>2230</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Tybee Island, GA</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t xml:space="preserve">xmas came early thank you #Bitcoin $BTC </t>
+          <t xml:space="preserve">RT @TribulationThe: TREASON by the Biden Crime Family!"Please Have Keys Made": Joe Biden Was Chinese Financier's "Office Mate" According… </t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>xmas came early  thank you #Bitcoin $BTC</t>
+          <t xml:space="preserve"> TREASON by the Biden Crime Family!  "Please Have Keys Made": Joe Biden Was Chinese Financier's "Office Mate" According…</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t xml:space="preserve">xmas came early thank you #Bitcoin $BTC </t>
+          <t xml:space="preserve"> TREASON by the Biden Crime Family!"Please Have Keys Made": Joe Biden Was Chinese Financier's "Office Mate" According… </t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t xml:space="preserve">xmas came early thank you #Bitcoin $BTC </t>
+          <t xml:space="preserve">RT @TribulationThe: TREASON by the Biden Crime Family!"Please Have Keys Made": Joe Biden Was Chinese Financier's "Office Mate" According… </t>
         </is>
       </c>
     </row>
@@ -568,53 +572,57 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>@Kneteknilch @mspro DIE Lösung für alles...Das habe ich auch nie behauptet. Dennoch wird Bitcoin nicht durch irgend… https://t.co/t6zfoL1WvH</t>
+          <t>Sen. Mitch McConnell: "Under President #Trump's command, our forces took terrorist leaders like Baghdadi &amp;amp;  Qasem S… https://t.co/LRH8KmSy2k</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.339281909587775e+18</v>
+        <v>1.33931361351388e+18</v>
       </c>
       <c r="D3" t="n">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44181.78546296297</v>
+        <v>44181.87295138889</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>de</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.311435962925429e+18</v>
+        <v>2343557479</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>HodlingSquirrel</t>
+          <t>MostafaMe4</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>6</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
+        <v>7816</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Europe</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t xml:space="preserve">@Kneteknilch @mspro THE solution for everything ... I never said that. Still, Bitcoin is not made by any ... https://t.co/t6zfoL1WvH </t>
+          <t xml:space="preserve">Sen. Mitch McConnell: "Under President #Trump's command, our forces took terrorist leaders like Baghdadi &amp;amp;  Qasem S… https://t.co/LRH8KmSy2k </t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  DIE Lösung für alles...Das habe ich auch nie behauptet. Dennoch wird Bitcoin nicht durch irgend… </t>
+          <t xml:space="preserve">Sen. Mitch McConnell: "Under President #Trump's command, our forces took terrorist leaders like Baghdadi &amp;amp;  Qasem S… </t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve">  THE solution for everything ... I never said that. Still, Bitcoin is not made by any ...  </t>
+          <t xml:space="preserve">Sen. Mitch McConnell: "Under President #Trump's command, our forces took terrorist leaders like Baghdadi &amp;amp;  Qasem S…  </t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t xml:space="preserve">@Kneteknilch @mspro THE solution for everything ... I never said that. Still, Bitcoin is not made by any ...  </t>
+          <t xml:space="preserve">Sen. Mitch McConnell: "Under President #Trump's command, our forces took terrorist leaders like Baghdadi &amp;amp;  Qasem S…  </t>
         </is>
       </c>
     </row>
@@ -624,17 +632,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>This truly aged well.  #Bitcoin https://t.co/2dgOjMAjJe</t>
+          <t>RT @yoksig: @SusanLynch22 @SuzieBird4 @Missin_Florida @skewermann @P4boxers @HeathenResister @openpodbaydoor_ @DearAuntCrabby @BlogChurchWo…</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.339281909512286e+18</v>
+        <v>1.339313610762445e+18</v>
       </c>
       <c r="D4" t="n">
-        <v>55</v>
+        <v>140</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44181.78546296297</v>
+        <v>44181.87293981481</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -642,39 +650,39 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>19603980</v>
+        <v>247054633</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>GlenACooper</t>
+          <t>jkf3500</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>101</v>
+        <v>25089</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Reston, VA</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t xml:space="preserve">This truly aged well.  #Bitcoin https://t.co/2dgOjMAjJe </t>
+          <t xml:space="preserve">RT @yoksig: @SusanLynch22 @SuzieBird4 @Missin_Florida @skewermann @P4boxers @HeathenResister @openpodbaydoor_ @DearAuntCrabby @BlogChurchWo… </t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve">This truly aged well.  #Bitcoin </t>
+          <t xml:space="preserve">         …</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve">This truly aged well.  #Bitcoin  </t>
+          <t xml:space="preserve">         … </t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t xml:space="preserve">This truly aged well.  #Bitcoin  </t>
+          <t xml:space="preserve">RT @yoksig: @SusanLynch22 @SuzieBird4 @Missin_Florida @skewermann @P4boxers @HeathenResister @openpodbaydoor_ @DearAuntCrabby @BlogChurchWo… </t>
         </is>
       </c>
     </row>
@@ -684,54 +692,53 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>#16Dic La policía de Trinidad y Tobago. maltratando y Agrediendo  a Migrantes Venezolanos 
- Es inaceptable que los… https://t.co/U9JJdOks6R</t>
+          <t>Nenhum dos repórteres na sala perguntou-lhe sobre o espião chinês no escritório de Eric Swalwell, então ela mesma f… https://t.co/ijmucNb4Ng</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.339281905062195e+18</v>
+        <v>1.339313569838588e+18</v>
       </c>
       <c r="D5" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>44181.78545138889</v>
+        <v>44181.87282407407</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>es</t>
+          <t>pt</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>430205402</v>
+        <v>128376943</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>VzlaUfo</t>
+          <t>German_Emanuel</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>2084</v>
+        <v>61</v>
       </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t xml:space="preserve"># 16Dec Trinidad and Tobago Police. mistreating and attacking Venezuelan Migrants It is unacceptable that the… https://t.co/U9JJdOks6R </t>
+          <t xml:space="preserve">None of the reporters in the room asked her about the Chinese spy at Eric Swalwell's office, so she herself… https://t.co/ijmucNb4Ng </t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t xml:space="preserve">#16Dic La policía de Trinidad y Tobago. maltratando y Agrediendo  a Migrantes Venezolanos   Es inaceptable que los… </t>
+          <t xml:space="preserve">Nenhum dos repórteres na sala perguntou-lhe sobre o espião chinês no escritório de Eric Swalwell, então ela mesma f… </t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t xml:space="preserve"># 16Dec Trinidad and Tobago Police. mistreating and attacking Venezuelan Migrants It is unacceptable that the…  </t>
+          <t xml:space="preserve">None of the reporters in the room asked her about the Chinese spy at Eric Swalwell's office, so she herself…  </t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t xml:space="preserve"># 16Dec Trinidad and Tobago Police. mistreating and attacking Venezuelan Migrants It is unacceptable that the…  </t>
+          <t xml:space="preserve">None of the reporters in the room asked her about the Chinese spy at Eric Swalwell's office, so she herself…  </t>
         </is>
       </c>
     </row>
@@ -741,17 +748,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin</t>
+          <t>Apparently Trump thought he was running against himself not against Biden. No, beating your own score doesn’t autom… https://t.co/89zD1fedtN</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1.339281902096634e+18</v>
+        <v>1.339313511420183e+18</v>
       </c>
       <c r="D6" t="n">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>44181.78543981481</v>
+        <v>44181.87267361111</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -759,39 +766,39 @@
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1.259302062434578e+18</v>
+        <v>1.017492973523698e+18</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>KOBOcrypto</t>
+          <t>RachelWilder_</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>14</v>
+        <v>229</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>California, USA</t>
+          <t>🌎</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin </t>
+          <t xml:space="preserve">Apparently Trump thought he was running against himself not against Biden. No, beating your own score doesn’t autom… https://t.co/89zD1fedtN </t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin</t>
+          <t xml:space="preserve">Apparently Trump thought he was running against himself not against Biden. No, beating your own score doesn’t autom… </t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin </t>
+          <t xml:space="preserve">Apparently Trump thought he was running against himself not against Biden. No, beating your own score doesn’t autom…  </t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Buy every dip. Buy every rumor. Hold through the news. Never sell. One day you won't need to. #Bitcoin </t>
+          <t xml:space="preserve">Apparently Trump thought he was running against himself not against Biden. No, beating your own score doesn’t autom…  </t>
         </is>
       </c>
     </row>
@@ -801,58 +808,57 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RT @davidnathan: Humeur du jour chez les bitcoiners... 😁 https://t.co/nZbOGMwFTT
-#Bitcoin #BTC</t>
+          <t>RT @AllenLEllison: .@StephenKing even you couldn’t have written a book more horrific than what #Trump has done to this country. #Rubio had…</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.33928190054067e+18</v>
+        <v>1.339313501899088e+18</v>
       </c>
       <c r="D7" t="n">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>44181.78543981481</v>
+        <v>44181.87263888889</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>fr</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>1.321825428974297e+18</v>
+        <v>2508838914</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>crypto_actu_fr</t>
+          <t>StuTheJanitor</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>130</v>
+        <v>4738</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t xml:space="preserve">France </t>
+          <t>Portland, OR</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @davidnathan: Mood of the day among bitcoiners ... 😁 https://t.co/nZbOGMwFTT#Bitcoin #BTC </t>
+          <t xml:space="preserve">RT @AllenLEllison: .@StephenKing even you couldn’t have written a book more horrific than what #Trump has done to this country. #Rubio had… </t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Humeur du jour chez les bitcoiners... 😁   #Bitcoin #BTC</t>
+          <t xml:space="preserve"> . even you couldn’t have written a book more horrific than what #Trump has done to this country. #Rubio had…</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Mood of the day among bitcoiners ... 😁 #Bitcoin #BTC </t>
+          <t xml:space="preserve"> . even you couldn’t have written a book more horrific than what #Trump has done to this country. #Rubio had… </t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @davidnathan: Mood of the day among bitcoiners ... 😁 #Bitcoin #BTC </t>
+          <t xml:space="preserve">RT @AllenLEllison: .@StephenKing even you couldn’t have written a book more horrific than what #Trump has done to this country. #Rubio had… </t>
         </is>
       </c>
     </row>
@@ -862,53 +868,53 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>@milyonerzihin @RealWorldCripto #Bitcoin 36500</t>
+          <t>RT @PdS1748: @Butterf70713546 @Dragonmaster969 @Boduoghnat @telegraaf Wat een geweldig artikel over de handelingen van #Trump. #TRUMP2020To…</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.339281895562023e+18</v>
+        <v>1.339313472287498e+18</v>
       </c>
       <c r="D8" t="n">
-        <v>46</v>
+        <v>140</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>44181.78542824074</v>
+        <v>44181.87255787037</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>und</t>
+          <t>nl</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>85309928</v>
+        <v>1.276310374669783e+18</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>r_tuynak</t>
+          <t>Rudy84529712</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>334</v>
+        <v>619</v>
       </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
-          <t xml:space="preserve">@milyonerzihin @RealWorldCripto #Bitcoin 36500 </t>
+          <t xml:space="preserve">RT @ PdS1748: @ Butterf70713546 @ Dragonmaster969 @Boduoghnat @telegraaf What a great article about the actions of #Trump. # TRUMP2020To ... </t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  #Bitcoin 36500</t>
+          <t xml:space="preserve">     Wat een geweldig artikel over de handelingen van #Trump. #TRUMP2020To…</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t xml:space="preserve">  #Bitcoin 36500 </t>
+          <t xml:space="preserve">RT  PdS1748:  Butterf70713546  Dragonmaster969 Boduoghnat telegraaf What a great article about the actions of #Trump. # TRUMP2020To ... </t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t xml:space="preserve">@milyonerzihin @RealWorldCripto #Bitcoin 36500 </t>
+          <t xml:space="preserve">RT @ PdS1748: @ Butterf70713546 @ Dragonmaster969 @Boduoghnat @telegraaf What a great article about the actions of #Trump. # TRUMP2020To ... </t>
         </is>
       </c>
     </row>
@@ -918,53 +924,53 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RT @jsblokland: BREAKING! #Bitcoin spikes to above USD 20,000! https://t.co/olLH68WW7W</t>
+          <t>#MAGA #Trump #Republicans #GOP #MitchMcConnell #Canada #StimulusCheckNOW #Stimuluscheck #JoseBiden #FoxNews #COVID19 https://t.co/gP6k3ATA2q</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.339281894827938e+18</v>
+        <v>1.339313444781093e+18</v>
       </c>
       <c r="D9" t="n">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>44181.78542824074</v>
+        <v>44181.87248842593</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>und</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>9.988576414546575e+17</v>
+        <v>1.337280942184878e+18</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Sonal913</t>
+          <t>cynthia26942734</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @jsblokland: BREAKING! #Bitcoin spikes to above USD 20,000! https://t.co/olLH68WW7W </t>
+          <t xml:space="preserve">#MAGA #Trump #Republicans #GOP #MitchMcConnell #Canada #StimulusCheckNOW #Stimuluscheck #JoseBiden #FoxNews #COVID19 https://t.co/gP6k3ATA2q </t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> BREAKING! #Bitcoin spikes to above USD 20,000! </t>
+          <t xml:space="preserve">#MAGA #Trump #Republicans #GOP #MitchMcConnell #Canada #StimulusCheckNOW #Stimuluscheck #JoseBiden #FoxNews #COVID19 </t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> BREAKING! #Bitcoin spikes to above USD 20,000!  </t>
+          <t xml:space="preserve">#MAGA #Trump #Republicans #GOP #MitchMcConnell #Canada #StimulusCheckNOW #Stimuluscheck #JoseBiden #FoxNews #COVID19  </t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @jsblokland: BREAKING! #Bitcoin spikes to above USD 20,000!  </t>
+          <t xml:space="preserve">#MAGA #Trump #Republicans #GOP #MitchMcConnell #Canada #StimulusCheckNOW #Stimuluscheck #JoseBiden #FoxNews #COVID19  </t>
         </is>
       </c>
     </row>
@@ -974,59 +980,57 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>RT @NamregNortlas: #16Dic
-#ANCSoberaniaYPaz
-#FelizMiercoles
-#BitCoin
-Día DEL Dibujante
-Copenhague
-#ExiliarAlReyYa #SOScolombiaddhh #Bolchev…</t>
+          <t>#Trump literally gave a foreign ENEMY state that has nuclear weapons pointed at us backdoor access into ALL governm… https://t.co/QGT9RpEjfK</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.339281892672205e+18</v>
+        <v>1.339313434664505e+18</v>
       </c>
       <c r="D10" t="n">
         <v>140</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>44181.78541666667</v>
+        <v>44181.87245370371</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>es</t>
+          <t>en</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1.318655859367547e+18</v>
+        <v>9.918115387125146e+17</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>DORISGa60466222</t>
+          <t>_Anonym0us_FL_</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>295</v>
-      </c>
-      <c r="J10" t="inlineStr"/>
+        <v>138</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Florida, USA</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @NamregNortlas: # 16Dec # ANCSoberaniaYPaz # FelizMiercoles # BitCoinDía DEL CartoonjaCopenhague # ExiliarAlReyYa #SOScolombiaddhh # Bolchev… </t>
+          <t xml:space="preserve">#Trump literally gave a foreign ENEMY state that has nuclear weapons pointed at us backdoor access into ALL governm… https://t.co/QGT9RpEjfK </t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> #16Dic #ANCSoberaniaYPaz #FelizMiercoles #BitCoin Día DEL Dibujante Copenhague #ExiliarAlReyYa #SOScolombiaddhh #Bolchev…</t>
+          <t xml:space="preserve">#Trump literally gave a foreign ENEMY state that has nuclear weapons pointed at us backdoor access into ALL governm… </t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> # 16Dec # ANCSoberaniaYPaz # FelizMiercoles # BitCoinDía DEL CartoonjaCopenhague # ExiliarAlReyYa #SOScolombiaddhh # Bolchev… </t>
+          <t xml:space="preserve">#Trump literally gave a foreign ENEMY state that has nuclear weapons pointed at us backdoor access into ALL governm…  </t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t xml:space="preserve">RT @NamregNortlas: # 16Dec # ANCSoberaniaYPaz # FelizMiercoles # BitCoinDía DEL CartoonjaCopenhague # ExiliarAlReyYa #SOScolombiaddhh # Bolchev… </t>
+          <t xml:space="preserve">#Trump literally gave a foreign ENEMY state that has nuclear weapons pointed at us backdoor access into ALL governm…  </t>
         </is>
       </c>
     </row>
@@ -1036,54 +1040,58 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The most important function of AITD chain is connecting the world!
- #Ethereum #bitcoin #eth #uniswap #defi #gem… https://t.co/1bBsek11Ui</t>
+          <t>President #Trump did in fact win the Election 
+فاکس نیوز هم اقرار به بُرد آقای ترامپ در انتخابات شد.… https://t.co/OdA7VTt2XE</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1.339281891392893e+18</v>
+        <v>1.339313427144012e+18</v>
       </c>
       <c r="D11" t="n">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>44181.78541666667</v>
+        <v>44181.87243055556</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>und</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>1.298076739369804e+18</v>
+        <v>9.723674191161467e+17</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>BlockchainAitd</t>
+          <t>Ali49781135</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>49</v>
-      </c>
-      <c r="J11" t="inlineStr"/>
+        <v>1094</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Iran,Tehran</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t xml:space="preserve">The most important function of AITD chain is connecting the world! #Ethereum #bitcoin #eth #uniswap #defi #gem… https://t.co/1bBsek11Ui </t>
+          <t xml:space="preserve">President #Trump did in fact win the Election Fox News also acknowledged Mr. Trump's victory in the election.… Https://t.co/OdA7VTt2XE </t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t xml:space="preserve">The most important function of AITD chain is connecting the world!  #Ethereum #bitcoin #eth #uniswap #defi #gem… </t>
+          <t xml:space="preserve">President #Trump did in fact win the Election  فاکس نیوز هم اقرار به بُرد آقای ترامپ در انتخابات شد.… </t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t xml:space="preserve">The most important function of AITD chain is connecting the world! #Ethereum #bitcoin #eth #uniswap #defi #gem…  </t>
+          <t xml:space="preserve">President #Trump did in fact win the Election Fox News also acknowledged Mr. Trump's victory in the election.… Https://t.co/OdA7VTt2XE </t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t xml:space="preserve">The most important function of AITD chain is connecting the world! #Ethereum #bitcoin #eth #uniswap #defi #gem…  </t>
+          <t xml:space="preserve">President #Trump did in fact win the Election Fox News also acknowledged Mr. Trump's victory in the election.… Https://t.co/OdA7VTt2XE </t>
         </is>
       </c>
     </row>

</xml_diff>